<commit_message>
Add xref and tweak timeline store
</commit_message>
<xml_diff>
--- a/source_data/profile_1.xlsx
+++ b/source_data/profile_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9CCD732-13FD-434B-81D2-6415FAF706CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422C6C92-DC60-E34A-AC5F-F75B7E31AAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="68220" yWindow="500" windowWidth="32180" windowHeight="26800" activeTab="4" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="studyIdentifiers" sheetId="3" r:id="rId2"/>
     <sheet name="studyDesign" sheetId="4" r:id="rId3"/>
     <sheet name="mainTimeline" sheetId="1" r:id="rId4"/>
-    <sheet name="profileTimeline" sheetId="11" r:id="rId5"/>
+    <sheet name="profile1" sheetId="11" r:id="rId5"/>
     <sheet name="studyDesignII" sheetId="6" r:id="rId6"/>
     <sheet name="studyDesignPopulations" sheetId="7" r:id="rId7"/>
     <sheet name="studyDesignOE" sheetId="8" r:id="rId8"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="196">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -611,9 +611,6 @@
     <t>otherTimelines</t>
   </si>
   <si>
-    <t>profileTimeline</t>
-  </si>
-  <si>
     <t>N: 1 Hour</t>
   </si>
   <si>
@@ -630,6 +627,12 @@
   </si>
   <si>
     <t>Temperature</t>
+  </si>
+  <si>
+    <t>PR:profile1</t>
+  </si>
+  <si>
+    <t>profile1</t>
   </si>
 </sst>
 </file>
@@ -1494,7 +1497,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:E7"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1586,7 +1589,7 @@
         <v>187</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -1675,7 +1678,7 @@
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="C29" sqref="C29"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1903,7 +1906,7 @@
         <v>29</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>28</v>
+        <v>194</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>9</v>
@@ -1939,7 +1942,7 @@
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomRight" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2070,19 +2073,19 @@
         <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -2145,10 +2148,10 @@
         <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>9</v>
@@ -2171,10 +2174,10 @@
         <v>28</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Add in timeline parameters
</commit_message>
<xml_diff>
--- a/source_data/profile_1.xlsx
+++ b/source_data/profile_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422C6C92-DC60-E34A-AC5F-F75B7E31AAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE585828-5EE1-5A45-ACBB-1092A4F4156D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="68220" yWindow="500" windowWidth="32180" windowHeight="26800" activeTab="4" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
@@ -45,10 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="196">
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="204">
   <si>
     <t>Epoch</t>
   </si>
@@ -633,6 +630,33 @@
   </si>
   <si>
     <t>profile1</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Profile One</t>
+  </si>
+  <si>
+    <t>A test profile</t>
+  </si>
+  <si>
+    <t>Main Timeline</t>
+  </si>
+  <si>
+    <t>This is the main timeline for the study design.</t>
+  </si>
+  <si>
+    <t>Potential subject identified</t>
+  </si>
+  <si>
+    <t>When activity executed</t>
   </si>
 </sst>
 </file>
@@ -704,7 +728,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -770,11 +794,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1109,10 +1142,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
@@ -1123,10 +1156,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
@@ -1137,10 +1170,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
@@ -1151,10 +1184,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
@@ -1165,10 +1198,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -1179,10 +1212,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -1193,10 +1226,10 @@
     </row>
     <row r="7" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" s="21" t="s">
         <v>167</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>168</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -1217,42 +1250,42 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="C9" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="D9" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="E9" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="F9" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="G9" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="H9" s="19" t="s">
         <v>158</v>
-      </c>
-      <c r="H9" s="19" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="C10" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="D10" s="14" t="s">
         <v>162</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>163</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -1262,33 +1295,33 @@
         <v>40179</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="C11" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>162</v>
-      </c>
       <c r="D11" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G11" s="20">
         <v>40544</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1391,18 +1424,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" t="s">
         <v>173</v>
-      </c>
-      <c r="B2" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1429,62 +1462,62 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>39</v>
-      </c>
       <c r="F1" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
         <v>40</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E2" t="s">
         <v>42</v>
       </c>
-      <c r="D2" t="s">
-        <v>184</v>
-      </c>
-      <c r="E2" t="s">
-        <v>43</v>
-      </c>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" t="s">
         <v>59</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E3" t="s">
         <v>60</v>
       </c>
-      <c r="D3" t="s">
-        <v>183</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>61</v>
-      </c>
-      <c r="F3" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1509,10 +1542,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -1520,10 +1553,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -1531,10 +1564,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -1542,10 +1575,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -1553,10 +1586,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
@@ -1564,10 +1597,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
@@ -1575,10 +1608,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
@@ -1586,10 +1619,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -1597,50 +1630,50 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>48</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1678,255 +1711,264 @@
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="28" style="3" customWidth="1"/>
     <col min="3" max="3" width="35.83203125" style="1" customWidth="1"/>
     <col min="4" max="8" width="12.33203125" style="1" customWidth="1"/>
     <col min="9" max="10" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="25"/>
+      <c r="H1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="F1" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="25"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="C9" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="C11" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B8"/>
+  <mergeCells count="1">
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1942,263 +1984,270 @@
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="C45" sqref="C45"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="25" style="3" customWidth="1"/>
     <col min="3" max="3" width="35.83203125" style="1" customWidth="1"/>
     <col min="4" max="8" width="12.33203125" style="1" customWidth="1"/>
     <col min="9" max="10" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="5" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
+      <c r="A2" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>199</v>
+      </c>
       <c r="C2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="5" t="s">
+      <c r="D5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="5" t="s">
+      <c r="D6" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="D7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="25"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="C9" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B8"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2219,72 +2268,72 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" t="s">
         <v>74</v>
-      </c>
-      <c r="D3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2311,72 +2360,72 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="D1" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
       <c r="C2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>83</v>
-      </c>
       <c r="E2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3">
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" t="s">
         <v>87</v>
-      </c>
-      <c r="E3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4">
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D4" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" t="s">
         <v>90</v>
-      </c>
-      <c r="E4" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2403,205 +2452,205 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="C1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>96</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="D2" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="E2" s="13" t="s">
+      <c r="G2" s="13" t="s">
         <v>100</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>104</v>
-      </c>
       <c r="G3" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
       <c r="D5" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
       <c r="D6" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F10" s="13"/>
       <c r="G10" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F12" s="13"/>
       <c r="G12" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
       <c r="D13" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -2814,90 +2863,90 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>138</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" t="s">
         <v>141</v>
       </c>
-      <c r="B2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>142</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H2" t="s">
         <v>143</v>
-      </c>
-      <c r="E2" t="s">
-        <v>147</v>
-      </c>
-      <c r="F2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G2" t="s">
-        <v>125</v>
-      </c>
-      <c r="H2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B5" t="s">
         <v>178</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D5" t="s">
         <v>179</v>
       </c>
-      <c r="C5" t="s">
-        <v>142</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>180</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G5" t="s">
+        <v>125</v>
+      </c>
+      <c r="H5" t="s">
         <v>181</v>
-      </c>
-      <c r="F5" t="s">
-        <v>120</v>
-      </c>
-      <c r="G5" t="s">
-        <v>126</v>
-      </c>
-      <c r="H5" t="s">
-        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add in timeline cross ref
</commit_message>
<xml_diff>
--- a/source_data/profile_1.xlsx
+++ b/source_data/profile_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE585828-5EE1-5A45-ACBB-1092A4F4156D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCCA1FA-6FC0-D742-9818-875691E6B574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68220" yWindow="500" windowWidth="32180" windowHeight="26800" activeTab="4" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="68220" yWindow="500" windowWidth="32180" windowHeight="26800" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -176,9 +176,6 @@
     <t>NCT12345678</t>
   </si>
   <si>
-    <t>Simple Test 1</t>
-  </si>
-  <si>
     <t>cell</t>
   </si>
   <si>
@@ -494,12 +491,6 @@
     <t>studyRationale</t>
   </si>
   <si>
-    <t>SIMPLE</t>
-  </si>
-  <si>
-    <t>A simple test</t>
-  </si>
-  <si>
     <t>briefTitle</t>
   </si>
   <si>
@@ -657,6 +648,15 @@
   </si>
   <si>
     <t>When activity executed</t>
+  </si>
+  <si>
+    <t>PROFILE TEST</t>
+  </si>
+  <si>
+    <t>Profile Test 1</t>
+  </si>
+  <si>
+    <t>A simple test of profiles</t>
   </si>
 </sst>
 </file>
@@ -1125,8 +1125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53AA772F-4124-4842-BA10-D27E5C5CE960}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1145,7 +1145,7 @@
         <v>29</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>43</v>
+        <v>202</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
@@ -1173,7 +1173,7 @@
         <v>31</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
@@ -1187,7 +1187,7 @@
         <v>32</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
@@ -1198,10 +1198,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>149</v>
+        <v>201</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -1212,10 +1212,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>150</v>
+        <v>203</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -1226,10 +1226,10 @@
     </row>
     <row r="7" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -1250,42 +1250,42 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="D9" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="E9" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="F9" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="G9" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="H9" s="19" t="s">
         <v>155</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="G9" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="H9" s="19" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="D10" s="14" t="s">
         <v>159</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>162</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -1295,33 +1295,33 @@
         <v>40179</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C11" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>161</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>164</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G11" s="20">
         <v>40544</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1424,18 +1424,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1477,7 +1477,7 @@
         <v>38</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1491,33 +1491,33 @@
         <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E2" t="s">
         <v>42</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" t="s">
         <v>58</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E3" t="s">
         <v>59</v>
       </c>
-      <c r="D3" t="s">
-        <v>182</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>60</v>
-      </c>
-      <c r="F3" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1542,10 +1542,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -1553,10 +1553,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -1564,10 +1564,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -1575,10 +1575,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -1586,10 +1586,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
@@ -1597,10 +1597,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
@@ -1608,10 +1608,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
@@ -1619,10 +1619,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -1630,7 +1630,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>13</v>
@@ -1639,41 +1639,41 @@
         <v>2</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1725,10 +1725,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
@@ -1744,15 +1744,15 @@
       </c>
       <c r="G1" s="25"/>
       <c r="H1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>3</v>
@@ -1775,10 +1775,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>23</v>
@@ -1923,7 +1923,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>8</v>
@@ -1949,7 +1949,7 @@
         <v>28</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>8</v>
@@ -1980,7 +1980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE8670E-14F5-DF47-B190-1E715EB319D4}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
@@ -1998,10 +1998,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" s="26" t="s">
         <v>195</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>198</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
@@ -2024,10 +2024,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>196</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>199</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>3</v>
@@ -2050,10 +2050,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>23</v>
@@ -2125,19 +2125,19 @@
         <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -2200,10 +2200,10 @@
         <v>27</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>8</v>
@@ -2226,10 +2226,10 @@
         <v>27</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>8</v>
@@ -2268,72 +2268,72 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" t="s">
         <v>73</v>
-      </c>
-      <c r="D3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2360,72 +2360,72 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>80</v>
-      </c>
       <c r="D1" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
       <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>82</v>
-      </c>
       <c r="E2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3">
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" t="s">
         <v>86</v>
-      </c>
-      <c r="E3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4">
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D4" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" t="s">
         <v>89</v>
-      </c>
-      <c r="E4" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2452,205 +2452,205 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>95</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="D2" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="E2" s="13" t="s">
+      <c r="G2" s="13" t="s">
         <v>99</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>103</v>
-      </c>
       <c r="G3" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
       <c r="D5" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
       <c r="D6" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F10" s="13"/>
       <c r="G10" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F12" s="13"/>
       <c r="G12" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
       <c r="D13" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -2863,90 +2863,90 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>137</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" t="s">
         <v>140</v>
       </c>
-      <c r="B2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>141</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" t="s">
         <v>142</v>
-      </c>
-      <c r="E2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G2" t="s">
-        <v>124</v>
-      </c>
-      <c r="H2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E5" t="s">
         <v>177</v>
       </c>
-      <c r="B5" t="s">
+      <c r="F5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G5" t="s">
+        <v>124</v>
+      </c>
+      <c r="H5" t="s">
         <v>178</v>
-      </c>
-      <c r="C5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D5" t="s">
-        <v>179</v>
-      </c>
-      <c r="E5" t="s">
-        <v>180</v>
-      </c>
-      <c r="F5" t="s">
-        <v>119</v>
-      </c>
-      <c r="G5" t="s">
-        <v>125</v>
-      </c>
-      <c r="H5" t="s">
-        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add in procedures, first cut
</commit_message>
<xml_diff>
--- a/source_data/profile_1.xlsx
+++ b/source_data/profile_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB77F3B6-C221-E54C-BC39-316E93C7394A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F772F08-2DD6-BB46-A2B7-9620E29995FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68200" yWindow="500" windowWidth="32180" windowHeight="26800" activeTab="3" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" activeTab="5" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -18,11 +18,12 @@
     <sheet name="studyDesign" sheetId="4" r:id="rId3"/>
     <sheet name="mainTimeline" sheetId="1" r:id="rId4"/>
     <sheet name="profile1" sheetId="11" r:id="rId5"/>
-    <sheet name="studyDesignII" sheetId="6" r:id="rId6"/>
-    <sheet name="studyDesignPopulations" sheetId="7" r:id="rId7"/>
-    <sheet name="studyDesignOE" sheetId="8" r:id="rId8"/>
-    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId9"/>
-    <sheet name="configuration" sheetId="10" r:id="rId10"/>
+    <sheet name="studyDesignProcedures" sheetId="12" r:id="rId6"/>
+    <sheet name="studyDesignII" sheetId="6" r:id="rId7"/>
+    <sheet name="studyDesignPopulations" sheetId="7" r:id="rId8"/>
+    <sheet name="studyDesignOE" sheetId="8" r:id="rId9"/>
+    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId10"/>
+    <sheet name="configuration" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="213">
   <si>
     <t>Epoch</t>
   </si>
@@ -617,9 +618,6 @@
     <t>Temperature</t>
   </si>
   <si>
-    <t>PR:profile1</t>
-  </si>
-  <si>
     <t>profile1</t>
   </si>
   <si>
@@ -657,6 +655,36 @@
   </si>
   <si>
     <t>A simple test of profiles</t>
+  </si>
+  <si>
+    <t>TL:profile1</t>
+  </si>
+  <si>
+    <t>procedureType</t>
+  </si>
+  <si>
+    <t>procedureCode</t>
+  </si>
+  <si>
+    <t>procedureIsConditional</t>
+  </si>
+  <si>
+    <t>procedureIsConditionalReason</t>
+  </si>
+  <si>
+    <t>XXX</t>
+  </si>
+  <si>
+    <t>PR1</t>
+  </si>
+  <si>
+    <t>SNOMED: 12345678=Test</t>
+  </si>
+  <si>
+    <t>PR2</t>
+  </si>
+  <si>
+    <t>SNOMED: 12345679=Test</t>
   </si>
 </sst>
 </file>
@@ -728,7 +756,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -785,6 +813,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -797,16 +837,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1126,7 +1157,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1145,7 +1176,7 @@
         <v>29</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
@@ -1201,7 +1232,7 @@
         <v>146</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -1215,7 +1246,7 @@
         <v>147</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -1410,6 +1441,117 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFC82B4-C495-A142-993D-B6A47D77A4C3}">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.83203125" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" customWidth="1"/>
+    <col min="6" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="61.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G5" t="s">
+        <v>124</v>
+      </c>
+      <c r="H5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1886B59F-3C17-014D-9C61-BEC33F421A82}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1544,89 +1686,89 @@
       <c r="A1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="26" t="s">
         <v>182</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="B8" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
+      <c r="B8" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
@@ -1690,14 +1832,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1707,11 +1849,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" sqref="A1:B3"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1724,11 +1866,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
-        <v>192</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>197</v>
+      <c r="A1" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>196</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
@@ -1739,20 +1881,20 @@
       <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="25"/>
+      <c r="G1" s="29"/>
       <c r="H1" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>198</v>
+      <c r="A2" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>197</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>3</v>
@@ -1774,11 +1916,11 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="27" t="s">
-        <v>194</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>199</v>
+      <c r="A3" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>198</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>23</v>
@@ -1800,8 +1942,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="5" t="s">
         <v>24</v>
       </c>
@@ -1822,8 +1964,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
       <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
@@ -1844,8 +1986,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="5" t="s">
         <v>25</v>
       </c>
@@ -1866,8 +2008,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
       <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
@@ -1888,8 +2030,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1949,7 +2091,7 @@
         <v>28</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>8</v>
@@ -1997,11 +2139,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
-        <v>192</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>195</v>
+      <c r="A1" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>194</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
@@ -2023,11 +2165,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>196</v>
+      <c r="A2" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>195</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>3</v>
@@ -2049,11 +2191,11 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="27" t="s">
-        <v>194</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>200</v>
+      <c r="A3" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>199</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>23</v>
@@ -2075,8 +2217,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="5" t="s">
         <v>24</v>
       </c>
@@ -2097,8 +2239,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
       <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
@@ -2119,8 +2261,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="5" t="s">
         <v>25</v>
       </c>
@@ -2141,8 +2283,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
       <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
@@ -2163,8 +2305,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="5" t="s">
         <v>7</v>
       </c>
@@ -2253,11 +2395,76 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7968437A-DBF9-A94D-B82A-825FF7E515F6}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>205</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E548DFC1-EB0E-374B-95D2-A04104B745FB}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2341,7 +2548,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C037A932-CB5B-8D43-956E-5F5C367E07FC}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -2433,7 +2640,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B908C5D6-C6A1-4043-A49A-69C599CFBAE9}">
   <dimension ref="A1:G36"/>
   <sheetViews>
@@ -2841,115 +3048,4 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFC82B4-C495-A142-993D-B6A47D77A4C3}">
-  <dimension ref="A1:H5"/>
-  <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="6.83203125" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="28.1640625" customWidth="1"/>
-    <col min="6" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="61.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G2" t="s">
-        <v>123</v>
-      </c>
-      <c r="H2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B5" t="s">
-        <v>175</v>
-      </c>
-      <c r="C5" t="s">
-        <v>140</v>
-      </c>
-      <c r="D5" t="s">
-        <v>176</v>
-      </c>
-      <c r="E5" t="s">
-        <v>177</v>
-      </c>
-      <c r="F5" t="s">
-        <v>118</v>
-      </c>
-      <c r="G5" t="s">
-        <v>124</v>
-      </c>
-      <c r="H5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>